<commit_message>
Correct glossary-entry "Nürnberger Gesetze"
</commit_message>
<xml_diff>
--- a/app/Resources/data/glossary.xlsx
+++ b/app/Resources/data/glossary.xlsx
@@ -1043,12 +1043,6 @@
     <t>Nürnberger Gesetze</t>
   </si>
   <si>
-    <t>„Gesetz zum Schutze des dt. Blutes und der dt. Ehre“ sowie „Gesetz über das Reichsbürgerrecht“. Sie verboten Eheschließungen und stellten den Geschlechtsverkehr zwischen „Ariern“ und „Nichtariern“</t>
-  </si>
-  <si>
-    <t>„Gesetz zum Schutze des dt. Blutes und der dt. Ehre“ sowie „Gesetz über das Reichsbürgerrecht“. Sie verboten Eheschließungen und stellten den Geschlechtsverkehr zwischen „Ariern“ und „Nichtariern“. In der Folge wurden Verordnungen erlassen, die die Einteilung in „Juden“ und „Mischlinge“ unterschiedlichen Grades regelten. Verabschiedet wurden dies Gesetze am 15.9.1935 auf dem Nürnberger Parteitag der NSDAP.</t>
-  </si>
-  <si>
     <t>Nuremberg Laws</t>
   </si>
   <si>
@@ -1502,6 +1496,12 @@
   </si>
   <si>
     <t>(Pl. Pauskim). Jüdischer Gelehrter (Dezisor), der bindende Entscheidung bei der Auslegung religiöser Gesetze ([[Halacha]]) trifft</t>
+  </si>
+  <si>
+    <t>„Gesetz zum Schutze des dt. Blutes und der dt. Ehre“ sowie „Gesetz über das Reichsbürgerrecht“. Sie verboten Eheschließungen und stellten den Geschlechtsverkehr zwischen „Ariern“ und „Nichtariern“ unter Strafe. In der Folge wurden Verordnungen erlassen, die die Einteilung in „Juden“ und „Mischlinge“ unterschiedlichen Grades regelten. Verabschiedet wurden dies Gesetze am 15.9.1935 auf dem Nürnberger Parteitag der NSDAP.</t>
+  </si>
+  <si>
+    <t>„Gesetz zum Schutze des dt. Blutes und der dt. Ehre“ sowie „Gesetz über das Reichsbürgerrecht“. Sie verboten Eheschließungen und stellten den Geschlechtsverkehr zwischen „Ariern“ und „Nichtariern“ unter Strafe</t>
   </si>
 </sst>
 </file>
@@ -1950,8 +1950,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F918"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B116" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D118" sqref="D118"/>
+    <sheetView tabSelected="1" topLeftCell="A111" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D113" sqref="D113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.3"/>
@@ -2012,7 +2012,7 @@
         <v>13</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="F3" s="3"/>
     </row>
@@ -2073,10 +2073,10 @@
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="3" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="F7" s="3"/>
     </row>
@@ -2128,7 +2128,7 @@
       </c>
       <c r="F10" s="7"/>
     </row>
-    <row r="11" spans="1:6" ht="271.7">
+    <row r="11" spans="1:6" ht="284.60000000000002">
       <c r="A11" s="5" t="s">
         <v>31</v>
       </c>
@@ -2252,7 +2252,7 @@
         <v>49</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="F18" s="5"/>
     </row>
@@ -2377,10 +2377,10 @@
       </c>
       <c r="C26" s="5"/>
       <c r="D26" s="3" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="F26" s="3"/>
     </row>
@@ -2891,7 +2891,7 @@
       </c>
       <c r="C58" s="5"/>
       <c r="D58" s="3" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="E58" s="3" t="s">
         <v>135</v>
@@ -3140,7 +3140,7 @@
       </c>
       <c r="F73" s="3"/>
     </row>
-    <row r="74" spans="1:6" ht="39.4">
+    <row r="74" spans="1:6" ht="52.3">
       <c r="A74" s="4" t="s">
         <v>175</v>
       </c>
@@ -3332,7 +3332,7 @@
       </c>
       <c r="F85" s="3"/>
     </row>
-    <row r="86" spans="1:6" ht="181.4">
+    <row r="86" spans="1:6" ht="194.3">
       <c r="A86" s="12" t="s">
         <v>201</v>
       </c>
@@ -3373,10 +3373,10 @@
       </c>
       <c r="C88" s="5"/>
       <c r="D88" s="3" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="E88" s="3" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="F88" s="4"/>
     </row>
@@ -3396,7 +3396,7 @@
       </c>
       <c r="F89" s="5"/>
     </row>
-    <row r="90" spans="1:6" ht="26.5">
+    <row r="90" spans="1:6" ht="39.4">
       <c r="A90" s="16" t="s">
         <v>209</v>
       </c>
@@ -3408,7 +3408,7 @@
         <v>210</v>
       </c>
       <c r="E90" s="3" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="F90" s="5"/>
     </row>
@@ -3572,7 +3572,7 @@
       </c>
       <c r="F100" s="3"/>
     </row>
-    <row r="101" spans="1:6" ht="39.4">
+    <row r="101" spans="1:6" ht="52.3">
       <c r="A101" t="s">
         <v>230</v>
       </c>
@@ -3654,7 +3654,7 @@
       </c>
       <c r="F105" s="10"/>
     </row>
-    <row r="106" spans="1:6" ht="303.64999999999998">
+    <row r="106" spans="1:6" ht="316.55">
       <c r="A106" s="17" t="s">
         <v>245</v>
       </c>
@@ -3727,10 +3727,10 @@
       </c>
       <c r="C110" s="5"/>
       <c r="D110" s="3" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="E110" s="3" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="F110" s="3"/>
     </row>
@@ -3775,860 +3775,860 @@
       </c>
       <c r="C113" s="1"/>
       <c r="D113" s="3" t="s">
+        <v>383</v>
+      </c>
+      <c r="E113" s="3" t="s">
+        <v>382</v>
+      </c>
+      <c r="F113" s="10"/>
+    </row>
+    <row r="114" spans="1:6" ht="116.85">
+      <c r="A114" s="20" t="s">
         <v>262</v>
-      </c>
-      <c r="E113" s="3" t="s">
-        <v>263</v>
-      </c>
-      <c r="F113" s="10"/>
-    </row>
-    <row r="114" spans="1:6" ht="116.85">
-      <c r="A114" s="14" t="s">
-        <v>264</v>
       </c>
       <c r="B114" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C114" s="5"/>
       <c r="D114" s="3" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="E114" s="3" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="F114" s="10"/>
     </row>
     <row r="115" spans="1:6" ht="78.150000000000006">
       <c r="A115" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B115" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C115" s="1"/>
       <c r="D115" s="3" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="E115" s="3" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="F115" s="4"/>
     </row>
     <row r="116" spans="1:6" ht="78.150000000000006">
       <c r="A116" s="4" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B116" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C116" s="5"/>
       <c r="D116" s="3" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="E116" s="3" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="F116" s="4"/>
     </row>
     <row r="117" spans="1:6" ht="39.4">
       <c r="A117" s="4" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="B117" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C117" s="5"/>
       <c r="D117" s="3" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="E117" s="3" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="F117" s="4"/>
     </row>
     <row r="118" spans="1:6" ht="39.4">
       <c r="A118" s="4" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="B118" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C118" s="5"/>
       <c r="D118" s="3" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="E118" s="3" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="F118" s="4"/>
     </row>
     <row r="119" spans="1:6" ht="52.3">
       <c r="A119" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B119" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C119" s="1"/>
       <c r="D119" s="3" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E119" s="3" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="F119" s="5"/>
     </row>
     <row r="120" spans="1:6" ht="52.3">
       <c r="A120" s="20" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="B120" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C120" s="5"/>
       <c r="D120" s="3" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E120" s="3" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="F120" s="5"/>
     </row>
     <row r="121" spans="1:6" ht="80.150000000000006">
       <c r="A121" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B121" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C121" s="1"/>
       <c r="D121" s="3" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="E121" s="3" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="F121" s="10"/>
     </row>
     <row r="122" spans="1:6" ht="65.25">
       <c r="A122" s="12" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="B122" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C122" s="5"/>
       <c r="D122" s="3" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="E122" s="3" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="F122" s="10"/>
     </row>
     <row r="123" spans="1:6" ht="39.4">
       <c r="A123" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B123" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C123" s="1"/>
       <c r="D123" s="3" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E123" s="3" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="F123" s="3"/>
     </row>
     <row r="124" spans="1:6" ht="39.4">
       <c r="A124" s="18" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B124" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C124" s="5"/>
       <c r="D124" s="3" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="E124" s="3" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="F124" s="3"/>
     </row>
-    <row r="125" spans="1:6" ht="65.25">
+    <row r="125" spans="1:6" ht="78.150000000000006">
       <c r="A125" s="1" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B125" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C125" s="1"/>
       <c r="D125" s="3" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="E125" s="3" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F125" s="3"/>
     </row>
     <row r="126" spans="1:6" ht="65.25">
       <c r="A126" s="12" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B126" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C126" s="5"/>
       <c r="D126" s="3" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="E126" s="3" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="F126" s="3"/>
     </row>
     <row r="127" spans="1:6" ht="39.4">
       <c r="A127" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B127" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C127" s="1"/>
       <c r="D127" s="3" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="E127" s="3" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="F127" s="4"/>
     </row>
     <row r="128" spans="1:6" ht="26.5">
       <c r="A128" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B128" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C128" s="5"/>
       <c r="D128" s="3" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="E128" s="3" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="F128" s="4"/>
     </row>
     <row r="129" spans="1:6">
       <c r="A129" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B129" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C129" s="1"/>
       <c r="D129" s="3" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="E129" s="3" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="F129" s="3"/>
     </row>
     <row r="130" spans="1:6">
       <c r="A130" s="4" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B130" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C130" s="5"/>
       <c r="D130" s="3" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="E130" s="3" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="F130" s="3"/>
     </row>
     <row r="131" spans="1:6">
       <c r="A131" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B131" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C131" s="1"/>
       <c r="D131" s="3" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="E131" s="3" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="F131" s="3"/>
     </row>
     <row r="132" spans="1:6">
       <c r="A132" s="4" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B132" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C132" s="5"/>
       <c r="D132" s="3" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="E132" s="3" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="F132" s="3"/>
     </row>
     <row r="133" spans="1:6" ht="91.05">
       <c r="A133" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B133" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C133" s="1"/>
       <c r="D133" s="3" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="E133" s="3" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="F133" s="11"/>
     </row>
     <row r="134" spans="1:6" ht="91.05">
       <c r="A134" s="12" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="B134" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C134" s="5"/>
       <c r="D134" s="3" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="E134" s="3" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="F134" s="11"/>
     </row>
     <row r="135" spans="1:6" ht="39.4">
       <c r="A135" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="B135" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C135" s="1"/>
       <c r="D135" s="3" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="E135" s="3" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="F135" s="3"/>
     </row>
     <row r="136" spans="1:6" ht="39.4">
       <c r="A136" s="4" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="B136" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C136" s="5"/>
       <c r="D136" s="3" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="E136" s="3" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="F136" s="3"/>
     </row>
     <row r="137" spans="1:6" ht="65.25">
       <c r="A137" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="B137" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C137" s="1"/>
       <c r="D137" s="3" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="E137" s="3" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="F137" s="3"/>
     </row>
     <row r="138" spans="1:6" ht="65.25">
       <c r="A138" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B138" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="D138" s="3" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="E138" s="3" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="F138" s="3"/>
     </row>
     <row r="139" spans="1:6">
       <c r="A139" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B139" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C139" s="1"/>
       <c r="D139" s="3" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E139" s="3" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="F139" s="3"/>
     </row>
     <row r="140" spans="1:6">
       <c r="A140" s="4" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B140" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C140" s="5"/>
       <c r="D140" s="3" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="E140" s="3" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="F140" s="3"/>
     </row>
     <row r="141" spans="1:6" ht="39.4">
       <c r="A141" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B141" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C141" s="1"/>
       <c r="D141" s="3" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="E141" s="3" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="F141" s="3"/>
     </row>
     <row r="142" spans="1:6" ht="39.4">
       <c r="A142" s="4" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="B142" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C142" s="5"/>
       <c r="D142" s="3" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="E142" s="3" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="F142" s="3"/>
     </row>
     <row r="143" spans="1:6" ht="26.5">
       <c r="A143" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B143" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C143" s="1"/>
       <c r="D143" s="3" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="E143" s="3" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="F143" s="4"/>
     </row>
     <row r="144" spans="1:6">
       <c r="A144" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B144" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C144" s="5"/>
       <c r="D144" s="3" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="E144" s="3" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="F144" s="4"/>
     </row>
     <row r="145" spans="1:6" ht="26.5">
       <c r="A145" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="B145" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C145" s="1"/>
       <c r="D145" s="3" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="E145" s="3" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="F145" s="3"/>
     </row>
     <row r="146" spans="1:6" ht="26.5">
       <c r="A146" s="4" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="B146" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C146" s="5"/>
       <c r="D146" s="3" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="E146" s="3" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="F146" s="3"/>
     </row>
     <row r="147" spans="1:6">
       <c r="A147" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B147" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C147" s="1"/>
       <c r="D147" s="3" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="E147" s="3" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="F147" s="3"/>
     </row>
     <row r="148" spans="1:6">
       <c r="A148" s="4" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B148" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C148" s="5"/>
       <c r="D148" s="3" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="E148" s="3" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="F148" s="3"/>
     </row>
     <row r="149" spans="1:6" ht="39.4">
       <c r="A149" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="B149" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C149" s="1"/>
       <c r="D149" s="3" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="E149" s="3" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="F149" s="3"/>
     </row>
     <row r="150" spans="1:6" ht="39.4">
       <c r="A150" s="4" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="B150" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C150" s="5"/>
       <c r="D150" s="3" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="E150" s="3" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="F150" s="3"/>
     </row>
     <row r="151" spans="1:6">
       <c r="A151" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="B151" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C151" s="1"/>
       <c r="D151" s="3" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="E151" s="3" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="F151" s="3"/>
     </row>
     <row r="152" spans="1:6" ht="26.5">
       <c r="A152" s="4" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="B152" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C152" s="5"/>
       <c r="D152" s="3" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="E152" s="3" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="F152" s="3"/>
     </row>
     <row r="153" spans="1:6">
       <c r="A153" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B153" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C153" s="1"/>
       <c r="D153" s="3" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="E153" s="3" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="F153" s="3"/>
     </row>
     <row r="154" spans="1:6">
       <c r="A154" s="4" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B154" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C154" s="5"/>
       <c r="D154" s="3" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="E154" s="3" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="F154" s="3"/>
     </row>
     <row r="155" spans="1:6" ht="52.3">
       <c r="A155" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="B155" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C155" s="1"/>
       <c r="D155" s="3" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="E155" s="3" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="F155" s="3"/>
     </row>
     <row r="156" spans="1:6" ht="52.3">
       <c r="A156" s="4" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="B156" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C156" s="5"/>
       <c r="D156" s="3" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="E156" s="3" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="F156" s="3"/>
     </row>
     <row r="157" spans="1:6" ht="142.65">
       <c r="A157" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B157" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C157" s="1"/>
       <c r="D157" s="3" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="E157" s="3" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="F157" s="11"/>
     </row>
     <row r="158" spans="1:6" ht="129.75">
       <c r="A158" s="4" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B158" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C158" s="5"/>
       <c r="D158" s="3" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="E158" s="3" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="F158" s="11"/>
     </row>
     <row r="159" spans="1:6" ht="26.5">
       <c r="A159" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="B159" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C159" s="1"/>
       <c r="D159" s="3" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="E159" s="3" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="F159" s="3"/>
     </row>
     <row r="160" spans="1:6" ht="26.5">
       <c r="A160" s="4" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="B160" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C160" s="5"/>
       <c r="D160" s="3" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="E160" s="3" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="F160" s="3"/>
     </row>
     <row r="161" spans="1:6" ht="26.5">
       <c r="A161" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="B161" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C161" s="1"/>
       <c r="D161" s="3" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="E161" s="3" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="F161" s="3"/>
     </row>
     <row r="162" spans="1:6" ht="26.5">
       <c r="A162" s="4" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="B162" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C162" s="5"/>
       <c r="D162" s="3" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="E162" s="3" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="F162" s="3"/>
     </row>
     <row r="163" spans="1:6" ht="78.150000000000006">
       <c r="A163" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="B163" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C163" s="1"/>
       <c r="D163" s="3" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="E163" s="3" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="F163" s="10"/>
     </row>
     <row r="164" spans="1:6" ht="67.25">
       <c r="A164" s="9" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="B164" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C164" s="5"/>
       <c r="D164" s="3" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="E164" s="3" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="F164" s="10"/>
     </row>
     <row r="165" spans="1:6">
       <c r="A165" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="B165" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C165" s="1"/>
       <c r="D165" s="3" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="E165" s="3" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="F165" s="4"/>
     </row>
     <row r="166" spans="1:6">
       <c r="A166" s="4" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="B166" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C166" s="5"/>
       <c r="D166" s="3" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="E166" s="3" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="F166" s="8"/>
     </row>

</xml_diff>

<commit_message>
Adjust sort if Person.givenName is null
</commit_message>
<xml_diff>
--- a/app/Resources/data/glossary.xlsx
+++ b/app/Resources/data/glossary.xlsx
@@ -499,30 +499,6 @@
   </si>
   <si>
     <t>Hakhshara(h)</t>
-  </si>
-  <si>
-    <r>
-      <t>This concept designates the regimen of mental and physical preparation for a life in Palestine. The movement developed at the end of the 19</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="10.5"/>
-        <color rgb="FF333333"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>th</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10.5"/>
-        <color rgb="FF333333"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> century, in so-called Hachshara centers knowledge was imparted concerning agriculture, artisan crafts and home economics, need in Palestine and for the building up of a kibbutz settlement. Most participants also resided in the Hachshara centers, studying Jewish history intensively and learning modern Hebrew.</t>
-    </r>
   </si>
   <si>
     <t>Halacha</t>
@@ -1503,12 +1479,36 @@
   <si>
     <t>„Gesetz zum Schutze des dt. Blutes und der dt. Ehre“ sowie „Gesetz über das Reichsbürgerrecht“. Sie verboten Eheschließungen und stellten den Geschlechtsverkehr zwischen „Ariern“ und „Nichtariern“ unter Strafe</t>
   </si>
+  <si>
+    <r>
+      <t>This concept designates the regimen of mental and physical preparation for a life in Palestine. The movement developed at the end of the 19</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10.5"/>
+        <color rgb="FF333333"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>th</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF333333"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> century, in so-called Hakhshara centers knowledge was imparted concerning agriculture, artisan crafts and home economics, need in Palestine and for the building up of a kibbutz settlement. Most participants also resided in the Hakhshara centers, studying Jewish history intensively and learning modern Hebrew.</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1576,6 +1576,12 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -1950,8 +1956,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F918"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A111" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D113" sqref="D113"/>
+    <sheetView tabSelected="1" topLeftCell="A56" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E58" sqref="E58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.3"/>
@@ -2012,7 +2018,7 @@
         <v>13</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="F3" s="3"/>
     </row>
@@ -2073,10 +2079,10 @@
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="3" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="F7" s="3"/>
     </row>
@@ -2128,7 +2134,7 @@
       </c>
       <c r="F10" s="7"/>
     </row>
-    <row r="11" spans="1:6" ht="284.60000000000002">
+    <row r="11" spans="1:6" ht="271.7">
       <c r="A11" s="5" t="s">
         <v>31</v>
       </c>
@@ -2252,7 +2258,7 @@
         <v>49</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="F18" s="5"/>
     </row>
@@ -2377,10 +2383,10 @@
       </c>
       <c r="C26" s="5"/>
       <c r="D26" s="3" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="F26" s="3"/>
     </row>
@@ -2891,1744 +2897,1744 @@
       </c>
       <c r="C58" s="5"/>
       <c r="D58" s="3" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>135</v>
+        <v>383</v>
       </c>
       <c r="F58" s="10"/>
     </row>
     <row r="59" spans="1:6" ht="26.5">
       <c r="A59" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C59" s="1"/>
       <c r="D59" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F59" s="3"/>
     </row>
     <row r="60" spans="1:6" ht="26.5">
       <c r="A60" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B60" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C60" s="5"/>
       <c r="D60" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F60" s="3"/>
     </row>
     <row r="61" spans="1:6">
       <c r="A61" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C61" s="1"/>
       <c r="D61" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E61" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F61" s="4"/>
     </row>
     <row r="62" spans="1:6">
       <c r="A62" s="12" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B62" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C62" s="5"/>
       <c r="D62" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E62" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F62" s="4"/>
     </row>
     <row r="63" spans="1:6" ht="91.05">
       <c r="A63" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C63" s="1"/>
       <c r="D63" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="E63" s="3" t="s">
         <v>145</v>
-      </c>
-      <c r="E63" s="3" t="s">
-        <v>146</v>
       </c>
       <c r="F63" s="10"/>
     </row>
     <row r="64" spans="1:6" ht="65.25">
       <c r="A64" s="12" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B64" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C64" s="5"/>
       <c r="D64" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="E64" s="3" t="s">
         <v>148</v>
-      </c>
-      <c r="E64" s="3" t="s">
-        <v>149</v>
       </c>
       <c r="F64" s="10"/>
     </row>
     <row r="65" spans="1:6" ht="26.5">
       <c r="A65" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C65" s="1"/>
       <c r="D65" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="E65" s="3" t="s">
         <v>151</v>
-      </c>
-      <c r="E65" s="3" t="s">
-        <v>152</v>
       </c>
       <c r="F65" s="3"/>
     </row>
     <row r="66" spans="1:6" ht="39.4">
       <c r="A66" s="4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B66" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C66" s="5"/>
       <c r="D66" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="E66" s="3" t="s">
         <v>154</v>
-      </c>
-      <c r="E66" s="3" t="s">
-        <v>155</v>
       </c>
       <c r="F66" s="3"/>
     </row>
     <row r="67" spans="1:6" ht="142.65">
       <c r="A67" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C67" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D67" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="D67" s="3" t="s">
+      <c r="E67" s="3" t="s">
         <v>158</v>
-      </c>
-      <c r="E67" s="3" t="s">
-        <v>159</v>
       </c>
       <c r="F67" s="10"/>
     </row>
     <row r="68" spans="1:6" ht="131.80000000000001">
       <c r="A68" s="6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B68" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C68" s="5"/>
       <c r="D68" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="E68" s="3" t="s">
         <v>161</v>
-      </c>
-      <c r="E68" s="3" t="s">
-        <v>162</v>
       </c>
       <c r="F68" s="10"/>
     </row>
     <row r="69" spans="1:6" ht="78.150000000000006">
       <c r="A69" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C69" s="1"/>
       <c r="D69" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="E69" s="3" t="s">
         <v>164</v>
-      </c>
-      <c r="E69" s="3" t="s">
-        <v>165</v>
       </c>
       <c r="F69" s="3"/>
     </row>
     <row r="70" spans="1:6" ht="65.25">
       <c r="A70" s="12" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B70" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C70" s="5"/>
       <c r="D70" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E70" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F70" s="3"/>
     </row>
     <row r="71" spans="1:6" ht="26.5">
       <c r="A71" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C71" s="1"/>
       <c r="D71" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E71" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F71" s="4"/>
     </row>
     <row r="72" spans="1:6" ht="26.5">
       <c r="A72" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B72" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C72" s="5"/>
       <c r="D72" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E72" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F72" s="4"/>
     </row>
     <row r="73" spans="1:6" ht="39.4">
       <c r="A73" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C73" s="1"/>
       <c r="D73" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="E73" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="E73" s="3" t="s">
+      <c r="F73" s="3"/>
+    </row>
+    <row r="74" spans="1:6" ht="39.4">
+      <c r="A74" s="4" t="s">
         <v>174</v>
-      </c>
-      <c r="F73" s="3"/>
-    </row>
-    <row r="74" spans="1:6" ht="52.3">
-      <c r="A74" s="4" t="s">
-        <v>175</v>
       </c>
       <c r="B74" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C74" s="5"/>
       <c r="D74" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E74" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F74" s="3"/>
     </row>
     <row r="75" spans="1:6">
       <c r="A75" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B75" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C75" s="1"/>
       <c r="D75" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E75" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F75" s="3"/>
     </row>
     <row r="76" spans="1:6">
       <c r="A76" s="6" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B76" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C76" s="5"/>
       <c r="D76" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E76" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F76" s="3"/>
     </row>
     <row r="77" spans="1:6" ht="26.5">
       <c r="A77" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B77" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C77" s="1"/>
       <c r="D77" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="E77" s="3" t="s">
         <v>181</v>
-      </c>
-      <c r="E77" s="3" t="s">
-        <v>182</v>
       </c>
       <c r="F77" s="10"/>
     </row>
     <row r="78" spans="1:6">
       <c r="A78" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B78" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C78" s="5"/>
       <c r="D78" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E78" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F78" s="10"/>
     </row>
     <row r="79" spans="1:6" ht="26.5">
       <c r="A79" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C79" s="1"/>
       <c r="D79" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E79" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F79" s="3"/>
     </row>
     <row r="80" spans="1:6" ht="26.5">
       <c r="A80" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B80" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C80" s="5"/>
       <c r="D80" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E80" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F80" s="3"/>
     </row>
     <row r="81" spans="1:6" ht="103.95">
       <c r="A81" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C81" s="1"/>
       <c r="D81" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="E81" s="3" t="s">
         <v>189</v>
-      </c>
-      <c r="E81" s="3" t="s">
-        <v>190</v>
       </c>
       <c r="F81" s="3"/>
     </row>
     <row r="82" spans="1:6" ht="103.95">
       <c r="A82" s="12" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B82" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C82" s="5"/>
       <c r="D82" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="E82" s="3" t="s">
         <v>192</v>
-      </c>
-      <c r="E82" s="3" t="s">
-        <v>193</v>
       </c>
       <c r="F82" s="3"/>
     </row>
     <row r="83" spans="1:6" ht="39.4">
       <c r="A83" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B83" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C83" s="1"/>
       <c r="D83" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="E83" s="3" t="s">
         <v>195</v>
-      </c>
-      <c r="E83" s="3" t="s">
-        <v>196</v>
       </c>
       <c r="F83" s="15"/>
     </row>
     <row r="84" spans="1:6" ht="26.5">
       <c r="A84" s="4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B84" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C84" s="5"/>
       <c r="D84" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E84" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F84" s="15"/>
     </row>
     <row r="85" spans="1:6" ht="220.1">
       <c r="A85" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B85" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C85" s="1"/>
       <c r="D85" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="E85" s="3" t="s">
         <v>199</v>
       </c>
-      <c r="E85" s="3" t="s">
+      <c r="F85" s="3"/>
+    </row>
+    <row r="86" spans="1:6" ht="181.4">
+      <c r="A86" s="12" t="s">
         <v>200</v>
-      </c>
-      <c r="F85" s="3"/>
-    </row>
-    <row r="86" spans="1:6" ht="194.3">
-      <c r="A86" s="12" t="s">
-        <v>201</v>
       </c>
       <c r="B86" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C86" s="5"/>
       <c r="D86" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="E86" s="3" t="s">
         <v>202</v>
-      </c>
-      <c r="E86" s="3" t="s">
-        <v>203</v>
       </c>
       <c r="F86" s="3"/>
     </row>
     <row r="87" spans="1:6">
       <c r="A87" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B87" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C87" s="1"/>
       <c r="D87" s="3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E87" s="3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="F87" s="4"/>
     </row>
     <row r="88" spans="1:6">
       <c r="A88" s="6" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B88" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C88" s="5"/>
       <c r="D88" s="3" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="E88" s="3" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="F88" s="4"/>
     </row>
     <row r="89" spans="1:6" ht="39.4">
       <c r="A89" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B89" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C89" s="1"/>
       <c r="D89" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="E89" s="3" t="s">
         <v>207</v>
       </c>
-      <c r="E89" s="3" t="s">
+      <c r="F89" s="5"/>
+    </row>
+    <row r="90" spans="1:6" ht="26.5">
+      <c r="A90" s="16" t="s">
         <v>208</v>
-      </c>
-      <c r="F89" s="5"/>
-    </row>
-    <row r="90" spans="1:6" ht="39.4">
-      <c r="A90" s="16" t="s">
-        <v>209</v>
       </c>
       <c r="B90" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C90" s="5"/>
       <c r="D90" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E90" s="3" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="F90" s="5"/>
     </row>
     <row r="91" spans="1:6">
       <c r="A91" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B91" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C91" s="1"/>
       <c r="D91" s="3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E91" s="3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F91" s="3"/>
     </row>
     <row r="92" spans="1:6">
       <c r="A92" s="4" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B92" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C92" s="5"/>
       <c r="D92" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E92" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F92" s="3"/>
     </row>
     <row r="93" spans="1:6" ht="26.5">
       <c r="A93" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B93" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C93" s="1"/>
       <c r="D93" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E93" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F93" s="3"/>
     </row>
     <row r="94" spans="1:6" ht="26.5">
       <c r="A94" s="4" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B94" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C94" s="5"/>
       <c r="D94" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E94" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F94" s="3"/>
     </row>
     <row r="95" spans="1:6">
       <c r="A95" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B95" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C95" s="1"/>
       <c r="D95" s="3" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E95" s="3" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F95" s="3"/>
     </row>
     <row r="96" spans="1:6">
       <c r="A96" s="4" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B96" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C96" s="5"/>
       <c r="D96" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E96" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F96" s="3"/>
     </row>
     <row r="97" spans="1:6">
       <c r="A97" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B97" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C97" s="1"/>
       <c r="D97" s="3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E97" s="3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F97" s="3"/>
     </row>
     <row r="98" spans="1:6">
       <c r="A98" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B98" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C98" s="5"/>
       <c r="D98" s="3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E98" s="3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F98" s="3"/>
     </row>
     <row r="99" spans="1:6" ht="39.4">
       <c r="A99" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B99" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C99" s="1"/>
       <c r="D99" s="3" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E99" s="3" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F99" s="3"/>
     </row>
     <row r="100" spans="1:6" ht="39.4">
       <c r="A100" s="4" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B100" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C100" s="5"/>
       <c r="D100" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="E100" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="F100" s="3"/>
+    </row>
+    <row r="101" spans="1:6" ht="39.4">
+      <c r="A101" t="s">
         <v>229</v>
-      </c>
-      <c r="E100" s="3" t="s">
-        <v>229</v>
-      </c>
-      <c r="F100" s="3"/>
-    </row>
-    <row r="101" spans="1:6" ht="52.3">
-      <c r="A101" t="s">
-        <v>230</v>
       </c>
       <c r="B101" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C101" s="1"/>
       <c r="D101" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="E101" s="3" t="s">
         <v>231</v>
-      </c>
-      <c r="E101" s="3" t="s">
-        <v>232</v>
       </c>
       <c r="F101" s="3"/>
     </row>
     <row r="102" spans="1:6" ht="52.3">
       <c r="A102" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B102" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C102" s="5"/>
       <c r="D102" s="3" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E102" s="3" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="F102" s="3"/>
     </row>
     <row r="103" spans="1:6" ht="310.45">
       <c r="A103" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B103" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C103" s="1"/>
       <c r="D103" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="E103" s="3" t="s">
         <v>236</v>
-      </c>
-      <c r="E103" s="3" t="s">
-        <v>237</v>
       </c>
       <c r="F103" s="10"/>
     </row>
     <row r="104" spans="1:6" ht="297.55">
       <c r="A104" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B104" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C104" s="5"/>
       <c r="D104" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="E104" s="3" t="s">
         <v>239</v>
-      </c>
-      <c r="E104" s="3" t="s">
-        <v>240</v>
       </c>
       <c r="F104" s="10"/>
     </row>
     <row r="105" spans="1:6" ht="323.35000000000002">
       <c r="A105" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B105" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C105" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="D105" s="3" t="s">
         <v>242</v>
       </c>
-      <c r="D105" s="3" t="s">
+      <c r="E105" s="3" t="s">
         <v>243</v>
       </c>
-      <c r="E105" s="3" t="s">
+      <c r="F105" s="10"/>
+    </row>
+    <row r="106" spans="1:6" ht="303.64999999999998">
+      <c r="A106" s="17" t="s">
         <v>244</v>
-      </c>
-      <c r="F105" s="10"/>
-    </row>
-    <row r="106" spans="1:6" ht="316.55">
-      <c r="A106" s="17" t="s">
-        <v>245</v>
       </c>
       <c r="B106" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C106" s="5"/>
       <c r="D106" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="E106" s="3" t="s">
         <v>246</v>
-      </c>
-      <c r="E106" s="3" t="s">
-        <v>247</v>
       </c>
       <c r="F106" s="10"/>
     </row>
     <row r="107" spans="1:6" ht="78.150000000000006">
       <c r="A107" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B107" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C107" s="1"/>
       <c r="D107" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="E107" s="3" t="s">
         <v>249</v>
-      </c>
-      <c r="E107" s="3" t="s">
-        <v>250</v>
       </c>
       <c r="F107" s="5"/>
     </row>
     <row r="108" spans="1:6" ht="65.25">
       <c r="A108" s="5" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B108" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C108" s="5"/>
       <c r="D108" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="E108" s="3" t="s">
         <v>252</v>
-      </c>
-      <c r="E108" s="3" t="s">
-        <v>253</v>
       </c>
       <c r="F108" s="5"/>
     </row>
     <row r="109" spans="1:6">
       <c r="A109" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B109" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C109" s="1"/>
       <c r="D109" s="3" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E109" s="3" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="F109" s="3"/>
     </row>
     <row r="110" spans="1:6">
       <c r="A110" s="6" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B110" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C110" s="5"/>
       <c r="D110" s="3" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="E110" s="3" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="F110" s="3"/>
     </row>
     <row r="111" spans="1:6">
       <c r="A111" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B111" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C111" s="1"/>
       <c r="D111" s="3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E111" s="3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="F111" s="3"/>
     </row>
     <row r="112" spans="1:6">
       <c r="A112" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B112" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C112" s="5"/>
       <c r="D112" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E112" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="F112" s="3"/>
     </row>
     <row r="113" spans="1:6" ht="142.65">
       <c r="A113" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B113" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C113" s="1"/>
       <c r="D113" s="3" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="E113" s="3" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="F113" s="10"/>
     </row>
     <row r="114" spans="1:6" ht="116.85">
       <c r="A114" s="20" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B114" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C114" s="5"/>
       <c r="D114" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="E114" s="3" t="s">
         <v>263</v>
-      </c>
-      <c r="E114" s="3" t="s">
-        <v>264</v>
       </c>
       <c r="F114" s="10"/>
     </row>
     <row r="115" spans="1:6" ht="78.150000000000006">
       <c r="A115" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B115" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C115" s="1"/>
       <c r="D115" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="E115" s="3" t="s">
         <v>266</v>
-      </c>
-      <c r="E115" s="3" t="s">
-        <v>267</v>
       </c>
       <c r="F115" s="4"/>
     </row>
     <row r="116" spans="1:6" ht="78.150000000000006">
       <c r="A116" s="4" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B116" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C116" s="5"/>
       <c r="D116" s="3" t="s">
+        <v>268</v>
+      </c>
+      <c r="E116" s="3" t="s">
         <v>269</v>
-      </c>
-      <c r="E116" s="3" t="s">
-        <v>270</v>
       </c>
       <c r="F116" s="4"/>
     </row>
     <row r="117" spans="1:6" ht="39.4">
       <c r="A117" s="4" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B117" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C117" s="5"/>
       <c r="D117" s="3" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="E117" s="3" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="F117" s="4"/>
     </row>
     <row r="118" spans="1:6" ht="39.4">
       <c r="A118" s="4" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B118" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C118" s="5"/>
       <c r="D118" s="3" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="E118" s="3" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="F118" s="4"/>
     </row>
     <row r="119" spans="1:6" ht="52.3">
       <c r="A119" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B119" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C119" s="1"/>
       <c r="D119" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="E119" s="3" t="s">
         <v>272</v>
-      </c>
-      <c r="E119" s="3" t="s">
-        <v>273</v>
       </c>
       <c r="F119" s="5"/>
     </row>
     <row r="120" spans="1:6" ht="52.3">
       <c r="A120" s="20" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B120" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C120" s="5"/>
       <c r="D120" s="3" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E120" s="3" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="F120" s="5"/>
     </row>
     <row r="121" spans="1:6" ht="80.150000000000006">
       <c r="A121" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B121" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C121" s="1"/>
       <c r="D121" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="E121" s="3" t="s">
         <v>277</v>
-      </c>
-      <c r="E121" s="3" t="s">
-        <v>278</v>
       </c>
       <c r="F121" s="10"/>
     </row>
     <row r="122" spans="1:6" ht="65.25">
       <c r="A122" s="12" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B122" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C122" s="5"/>
       <c r="D122" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="E122" s="3" t="s">
         <v>280</v>
-      </c>
-      <c r="E122" s="3" t="s">
-        <v>281</v>
       </c>
       <c r="F122" s="10"/>
     </row>
     <row r="123" spans="1:6" ht="39.4">
       <c r="A123" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B123" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C123" s="1"/>
       <c r="D123" s="3" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="E123" s="3" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="F123" s="3"/>
     </row>
     <row r="124" spans="1:6" ht="39.4">
       <c r="A124" s="18" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B124" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C124" s="5"/>
       <c r="D124" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="E124" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="F124" s="3"/>
+    </row>
+    <row r="125" spans="1:6" ht="65.25">
+      <c r="A125" s="1" t="s">
         <v>284</v>
-      </c>
-      <c r="E124" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="F124" s="3"/>
-    </row>
-    <row r="125" spans="1:6" ht="78.150000000000006">
-      <c r="A125" s="1" t="s">
-        <v>285</v>
       </c>
       <c r="B125" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C125" s="1"/>
       <c r="D125" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="E125" s="3" t="s">
         <v>286</v>
-      </c>
-      <c r="E125" s="3" t="s">
-        <v>287</v>
       </c>
       <c r="F125" s="3"/>
     </row>
     <row r="126" spans="1:6" ht="65.25">
       <c r="A126" s="12" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B126" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C126" s="5"/>
       <c r="D126" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="E126" s="3" t="s">
         <v>289</v>
-      </c>
-      <c r="E126" s="3" t="s">
-        <v>290</v>
       </c>
       <c r="F126" s="3"/>
     </row>
     <row r="127" spans="1:6" ht="39.4">
       <c r="A127" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B127" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C127" s="1"/>
       <c r="D127" s="3" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="E127" s="3" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="F127" s="4"/>
     </row>
     <row r="128" spans="1:6" ht="26.5">
       <c r="A128" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B128" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C128" s="5"/>
       <c r="D128" s="3" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="E128" s="3" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F128" s="4"/>
     </row>
     <row r="129" spans="1:6">
       <c r="A129" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B129" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C129" s="1"/>
       <c r="D129" s="3" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E129" s="3" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="F129" s="3"/>
     </row>
     <row r="130" spans="1:6">
       <c r="A130" s="4" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B130" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C130" s="5"/>
       <c r="D130" s="3" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="E130" s="3" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="F130" s="3"/>
     </row>
     <row r="131" spans="1:6">
       <c r="A131" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B131" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C131" s="1"/>
       <c r="D131" s="3" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="E131" s="3" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="F131" s="3"/>
     </row>
     <row r="132" spans="1:6">
       <c r="A132" s="4" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B132" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C132" s="5"/>
       <c r="D132" s="3" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="E132" s="3" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="F132" s="3"/>
     </row>
     <row r="133" spans="1:6" ht="91.05">
       <c r="A133" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B133" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C133" s="1"/>
       <c r="D133" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="E133" s="3" t="s">
         <v>303</v>
-      </c>
-      <c r="E133" s="3" t="s">
-        <v>304</v>
       </c>
       <c r="F133" s="11"/>
     </row>
     <row r="134" spans="1:6" ht="91.05">
       <c r="A134" s="12" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B134" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C134" s="5"/>
       <c r="D134" s="3" t="s">
+        <v>305</v>
+      </c>
+      <c r="E134" s="3" t="s">
         <v>306</v>
-      </c>
-      <c r="E134" s="3" t="s">
-        <v>307</v>
       </c>
       <c r="F134" s="11"/>
     </row>
     <row r="135" spans="1:6" ht="39.4">
       <c r="A135" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B135" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C135" s="1"/>
       <c r="D135" s="3" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="E135" s="3" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F135" s="3"/>
     </row>
     <row r="136" spans="1:6" ht="39.4">
       <c r="A136" s="4" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B136" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C136" s="5"/>
       <c r="D136" s="3" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E136" s="3" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F136" s="3"/>
     </row>
     <row r="137" spans="1:6" ht="65.25">
       <c r="A137" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B137" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C137" s="1"/>
       <c r="D137" s="3" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="E137" s="3" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="F137" s="3"/>
     </row>
     <row r="138" spans="1:6" ht="65.25">
       <c r="A138" s="1" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B138" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D138" s="3" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="E138" s="3" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="F138" s="3"/>
     </row>
     <row r="139" spans="1:6">
       <c r="A139" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B139" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C139" s="1"/>
       <c r="D139" s="3" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E139" s="3" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="F139" s="3"/>
     </row>
     <row r="140" spans="1:6">
       <c r="A140" s="4" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B140" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C140" s="5"/>
       <c r="D140" s="3" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="E140" s="3" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="F140" s="3"/>
     </row>
     <row r="141" spans="1:6" ht="39.4">
       <c r="A141" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B141" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C141" s="1"/>
       <c r="D141" s="3" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E141" s="3" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="F141" s="3"/>
     </row>
     <row r="142" spans="1:6" ht="39.4">
       <c r="A142" s="4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B142" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C142" s="5"/>
       <c r="D142" s="3" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="E142" s="3" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="F142" s="3"/>
     </row>
     <row r="143" spans="1:6" ht="26.5">
       <c r="A143" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B143" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C143" s="1"/>
       <c r="D143" s="3" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="E143" s="3" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="F143" s="4"/>
     </row>
     <row r="144" spans="1:6">
       <c r="A144" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B144" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C144" s="5"/>
       <c r="D144" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="E144" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="F144" s="4"/>
     </row>
     <row r="145" spans="1:6" ht="26.5">
       <c r="A145" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B145" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C145" s="1"/>
       <c r="D145" s="3" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="E145" s="3" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="F145" s="3"/>
     </row>
     <row r="146" spans="1:6" ht="26.5">
       <c r="A146" s="4" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B146" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C146" s="5"/>
       <c r="D146" s="3" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="E146" s="3" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="F146" s="3"/>
     </row>
     <row r="147" spans="1:6">
       <c r="A147" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B147" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C147" s="1"/>
       <c r="D147" s="3" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="E147" s="3" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="F147" s="3"/>
     </row>
     <row r="148" spans="1:6">
       <c r="A148" s="4" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B148" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C148" s="5"/>
       <c r="D148" s="3" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="E148" s="3" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="F148" s="3"/>
     </row>
     <row r="149" spans="1:6" ht="39.4">
       <c r="A149" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B149" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C149" s="1"/>
       <c r="D149" s="3" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E149" s="3" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="F149" s="3"/>
     </row>
     <row r="150" spans="1:6" ht="39.4">
       <c r="A150" s="4" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B150" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C150" s="5"/>
       <c r="D150" s="3" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="E150" s="3" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="F150" s="3"/>
     </row>
     <row r="151" spans="1:6">
       <c r="A151" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B151" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C151" s="1"/>
       <c r="D151" s="3" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E151" s="3" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="F151" s="3"/>
     </row>
     <row r="152" spans="1:6" ht="26.5">
       <c r="A152" s="4" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B152" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C152" s="5"/>
       <c r="D152" s="3" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E152" s="3" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="F152" s="3"/>
     </row>
     <row r="153" spans="1:6">
       <c r="A153" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B153" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C153" s="1"/>
       <c r="D153" s="3" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="E153" s="3" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="F153" s="3"/>
     </row>
     <row r="154" spans="1:6">
       <c r="A154" s="4" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B154" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C154" s="5"/>
       <c r="D154" s="3" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="E154" s="3" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="F154" s="3"/>
     </row>
     <row r="155" spans="1:6" ht="52.3">
       <c r="A155" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B155" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C155" s="1"/>
       <c r="D155" s="3" t="s">
+        <v>342</v>
+      </c>
+      <c r="E155" s="3" t="s">
         <v>343</v>
-      </c>
-      <c r="E155" s="3" t="s">
-        <v>344</v>
       </c>
       <c r="F155" s="3"/>
     </row>
     <row r="156" spans="1:6" ht="52.3">
       <c r="A156" s="4" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B156" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C156" s="5"/>
       <c r="D156" s="3" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="E156" s="3" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="F156" s="3"/>
     </row>
     <row r="157" spans="1:6" ht="142.65">
       <c r="A157" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B157" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C157" s="1"/>
       <c r="D157" s="3" t="s">
+        <v>347</v>
+      </c>
+      <c r="E157" s="3" t="s">
         <v>348</v>
-      </c>
-      <c r="E157" s="3" t="s">
-        <v>349</v>
       </c>
       <c r="F157" s="11"/>
     </row>
     <row r="158" spans="1:6" ht="129.75">
       <c r="A158" s="4" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B158" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C158" s="5"/>
       <c r="D158" s="3" t="s">
+        <v>349</v>
+      </c>
+      <c r="E158" s="3" t="s">
         <v>350</v>
-      </c>
-      <c r="E158" s="3" t="s">
-        <v>351</v>
       </c>
       <c r="F158" s="11"/>
     </row>
     <row r="159" spans="1:6" ht="26.5">
       <c r="A159" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B159" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C159" s="1"/>
       <c r="D159" s="3" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="E159" s="3" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="F159" s="3"/>
     </row>
     <row r="160" spans="1:6" ht="26.5">
       <c r="A160" s="4" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B160" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C160" s="5"/>
       <c r="D160" s="3" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E160" s="3" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F160" s="3"/>
     </row>
     <row r="161" spans="1:6" ht="26.5">
       <c r="A161" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B161" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C161" s="1"/>
       <c r="D161" s="3" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="E161" s="3" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="F161" s="3"/>
     </row>
     <row r="162" spans="1:6" ht="26.5">
       <c r="A162" s="4" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B162" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C162" s="5"/>
       <c r="D162" s="3" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="E162" s="3" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="F162" s="3"/>
     </row>
     <row r="163" spans="1:6" ht="78.150000000000006">
       <c r="A163" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B163" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C163" s="1"/>
       <c r="D163" s="3" t="s">
+        <v>359</v>
+      </c>
+      <c r="E163" s="3" t="s">
         <v>360</v>
-      </c>
-      <c r="E163" s="3" t="s">
-        <v>361</v>
       </c>
       <c r="F163" s="10"/>
     </row>
     <row r="164" spans="1:6" ht="67.25">
       <c r="A164" s="9" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B164" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C164" s="5"/>
       <c r="D164" s="3" t="s">
+        <v>362</v>
+      </c>
+      <c r="E164" s="3" t="s">
         <v>363</v>
-      </c>
-      <c r="E164" s="3" t="s">
-        <v>364</v>
       </c>
       <c r="F164" s="10"/>
     </row>
     <row r="165" spans="1:6">
       <c r="A165" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B165" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C165" s="1"/>
       <c r="D165" s="3" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="E165" s="3" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="F165" s="4"/>
     </row>
     <row r="166" spans="1:6">
       <c r="A166" s="4" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B166" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C166" s="5"/>
       <c r="D166" s="3" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="E166" s="3" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="F166" s="8"/>
     </row>
@@ -8393,6 +8399,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>